<commit_message>
Final versions of notebooks
</commit_message>
<xml_diff>
--- a/Resources/Clean/Clean_ParkData.xlsx
+++ b/Resources/Clean/Clean_ParkData.xlsx
@@ -12175,10 +12175,10 @@
         <v>56</v>
       </c>
       <c r="G284">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H284">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I284" t="s">
         <v>45</v>
@@ -12216,10 +12216,10 @@
         <v>56</v>
       </c>
       <c r="G285">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H285">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I285" t="s">
         <v>45</v>
@@ -12257,10 +12257,10 @@
         <v>56</v>
       </c>
       <c r="G286">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H286">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I286" t="s">
         <v>45</v>
@@ -12298,10 +12298,10 @@
         <v>56</v>
       </c>
       <c r="G287">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H287">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I287" t="s">
         <v>45</v>
@@ -12339,10 +12339,10 @@
         <v>56</v>
       </c>
       <c r="G288">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H288">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I288" t="s">
         <v>45</v>
@@ -12380,10 +12380,10 @@
         <v>56</v>
       </c>
       <c r="G289">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H289">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I289" t="s">
         <v>45</v>
@@ -12421,10 +12421,10 @@
         <v>56</v>
       </c>
       <c r="G290">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H290">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I290" t="s">
         <v>45</v>
@@ -12462,10 +12462,10 @@
         <v>56</v>
       </c>
       <c r="G291">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H291">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I291" t="s">
         <v>45</v>
@@ -12503,10 +12503,10 @@
         <v>56</v>
       </c>
       <c r="G292">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H292">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I292" t="s">
         <v>45</v>
@@ -12544,10 +12544,10 @@
         <v>56</v>
       </c>
       <c r="G293">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H293">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I293" t="s">
         <v>45</v>
@@ -12585,10 +12585,10 @@
         <v>56</v>
       </c>
       <c r="G294">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H294">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I294" t="s">
         <v>45</v>
@@ -12626,10 +12626,10 @@
         <v>56</v>
       </c>
       <c r="G295">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H295">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I295" t="s">
         <v>45</v>
@@ -12667,10 +12667,10 @@
         <v>56</v>
       </c>
       <c r="G296">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H296">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I296" t="s">
         <v>45</v>
@@ -12708,10 +12708,10 @@
         <v>56</v>
       </c>
       <c r="G297">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H297">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I297" t="s">
         <v>45</v>
@@ -12749,10 +12749,10 @@
         <v>56</v>
       </c>
       <c r="G298">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H298">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I298" t="s">
         <v>45</v>
@@ -12790,10 +12790,10 @@
         <v>56</v>
       </c>
       <c r="G299">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H299">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I299" t="s">
         <v>45</v>
@@ -12831,10 +12831,10 @@
         <v>56</v>
       </c>
       <c r="G300">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H300">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I300" t="s">
         <v>45</v>
@@ -12872,10 +12872,10 @@
         <v>56</v>
       </c>
       <c r="G301">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H301">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I301" t="s">
         <v>45</v>
@@ -12913,10 +12913,10 @@
         <v>56</v>
       </c>
       <c r="G302">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H302">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I302" t="s">
         <v>45</v>
@@ -12954,10 +12954,10 @@
         <v>56</v>
       </c>
       <c r="G303">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H303">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I303" t="s">
         <v>45</v>
@@ -12995,10 +12995,10 @@
         <v>56</v>
       </c>
       <c r="G304">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H304">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I304" t="s">
         <v>45</v>
@@ -13036,10 +13036,10 @@
         <v>56</v>
       </c>
       <c r="G305">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H305">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I305" t="s">
         <v>45</v>
@@ -13077,10 +13077,10 @@
         <v>56</v>
       </c>
       <c r="G306">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H306">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I306" t="s">
         <v>45</v>
@@ -13118,10 +13118,10 @@
         <v>56</v>
       </c>
       <c r="G307">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H307">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I307" t="s">
         <v>45</v>
@@ -13159,10 +13159,10 @@
         <v>56</v>
       </c>
       <c r="G308">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H308">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I308" t="s">
         <v>45</v>
@@ -13200,10 +13200,10 @@
         <v>56</v>
       </c>
       <c r="G309">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H309">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I309" t="s">
         <v>45</v>
@@ -13241,10 +13241,10 @@
         <v>56</v>
       </c>
       <c r="G310">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H310">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I310" t="s">
         <v>45</v>
@@ -13282,10 +13282,10 @@
         <v>56</v>
       </c>
       <c r="G311">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H311">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I311" t="s">
         <v>45</v>
@@ -13323,10 +13323,10 @@
         <v>56</v>
       </c>
       <c r="G312">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H312">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I312" t="s">
         <v>45</v>
@@ -13364,10 +13364,10 @@
         <v>56</v>
       </c>
       <c r="G313">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H313">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I313" t="s">
         <v>45</v>
@@ -13405,10 +13405,10 @@
         <v>56</v>
       </c>
       <c r="G314">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H314">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I314" t="s">
         <v>45</v>
@@ -13446,10 +13446,10 @@
         <v>56</v>
       </c>
       <c r="G315">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H315">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I315" t="s">
         <v>45</v>
@@ -13487,10 +13487,10 @@
         <v>56</v>
       </c>
       <c r="G316">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H316">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I316" t="s">
         <v>45</v>
@@ -13528,10 +13528,10 @@
         <v>56</v>
       </c>
       <c r="G317">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H317">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I317" t="s">
         <v>45</v>
@@ -13569,10 +13569,10 @@
         <v>56</v>
       </c>
       <c r="G318">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H318">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I318" t="s">
         <v>45</v>
@@ -13610,10 +13610,10 @@
         <v>56</v>
       </c>
       <c r="G319">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H319">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I319" t="s">
         <v>45</v>
@@ -13651,10 +13651,10 @@
         <v>56</v>
       </c>
       <c r="G320">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H320">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I320" t="s">
         <v>45</v>
@@ -13692,10 +13692,10 @@
         <v>56</v>
       </c>
       <c r="G321">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H321">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I321" t="s">
         <v>45</v>
@@ -13733,10 +13733,10 @@
         <v>56</v>
       </c>
       <c r="G322">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H322">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I322" t="s">
         <v>45</v>
@@ -13774,10 +13774,10 @@
         <v>56</v>
       </c>
       <c r="G323">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H323">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I323" t="s">
         <v>45</v>
@@ -13815,10 +13815,10 @@
         <v>56</v>
       </c>
       <c r="G324">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H324">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I324" t="s">
         <v>45</v>
@@ -13856,10 +13856,10 @@
         <v>56</v>
       </c>
       <c r="G325">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H325">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I325" t="s">
         <v>45</v>
@@ -13897,10 +13897,10 @@
         <v>56</v>
       </c>
       <c r="G326">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H326">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I326" t="s">
         <v>45</v>
@@ -13938,10 +13938,10 @@
         <v>56</v>
       </c>
       <c r="G327">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H327">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I327" t="s">
         <v>45</v>
@@ -13979,10 +13979,10 @@
         <v>56</v>
       </c>
       <c r="G328">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H328">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I328" t="s">
         <v>45</v>
@@ -14020,10 +14020,10 @@
         <v>56</v>
       </c>
       <c r="G329">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H329">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I329" t="s">
         <v>45</v>
@@ -14061,10 +14061,10 @@
         <v>56</v>
       </c>
       <c r="G330">
-        <v>46.8799663</v>
+        <v>46.85230749999999</v>
       </c>
       <c r="H330">
-        <v>-121.7269094</v>
+        <v>-121.7603229</v>
       </c>
       <c r="I330" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Repo Clean Up + Final Presentation
</commit_message>
<xml_diff>
--- a/Resources/Clean/Clean_ParkData.xlsx
+++ b/Resources/Clean/Clean_ParkData.xlsx
@@ -12175,10 +12175,10 @@
         <v>56</v>
       </c>
       <c r="G284">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H284">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I284" t="s">
         <v>45</v>
@@ -12216,10 +12216,10 @@
         <v>56</v>
       </c>
       <c r="G285">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H285">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I285" t="s">
         <v>45</v>
@@ -12257,10 +12257,10 @@
         <v>56</v>
       </c>
       <c r="G286">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H286">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I286" t="s">
         <v>45</v>
@@ -12298,10 +12298,10 @@
         <v>56</v>
       </c>
       <c r="G287">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H287">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I287" t="s">
         <v>45</v>
@@ -12339,10 +12339,10 @@
         <v>56</v>
       </c>
       <c r="G288">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H288">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I288" t="s">
         <v>45</v>
@@ -12380,10 +12380,10 @@
         <v>56</v>
       </c>
       <c r="G289">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H289">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I289" t="s">
         <v>45</v>
@@ -12421,10 +12421,10 @@
         <v>56</v>
       </c>
       <c r="G290">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H290">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I290" t="s">
         <v>45</v>
@@ -12462,10 +12462,10 @@
         <v>56</v>
       </c>
       <c r="G291">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H291">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I291" t="s">
         <v>45</v>
@@ -12503,10 +12503,10 @@
         <v>56</v>
       </c>
       <c r="G292">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H292">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I292" t="s">
         <v>45</v>
@@ -12544,10 +12544,10 @@
         <v>56</v>
       </c>
       <c r="G293">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H293">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I293" t="s">
         <v>45</v>
@@ -12585,10 +12585,10 @@
         <v>56</v>
       </c>
       <c r="G294">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H294">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I294" t="s">
         <v>45</v>
@@ -12626,10 +12626,10 @@
         <v>56</v>
       </c>
       <c r="G295">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H295">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I295" t="s">
         <v>45</v>
@@ -12667,10 +12667,10 @@
         <v>56</v>
       </c>
       <c r="G296">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H296">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I296" t="s">
         <v>45</v>
@@ -12708,10 +12708,10 @@
         <v>56</v>
       </c>
       <c r="G297">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H297">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I297" t="s">
         <v>45</v>
@@ -12749,10 +12749,10 @@
         <v>56</v>
       </c>
       <c r="G298">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H298">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I298" t="s">
         <v>45</v>
@@ -12790,10 +12790,10 @@
         <v>56</v>
       </c>
       <c r="G299">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H299">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I299" t="s">
         <v>45</v>
@@ -12831,10 +12831,10 @@
         <v>56</v>
       </c>
       <c r="G300">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H300">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I300" t="s">
         <v>45</v>
@@ -12872,10 +12872,10 @@
         <v>56</v>
       </c>
       <c r="G301">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H301">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I301" t="s">
         <v>45</v>
@@ -12913,10 +12913,10 @@
         <v>56</v>
       </c>
       <c r="G302">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H302">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I302" t="s">
         <v>45</v>
@@ -12954,10 +12954,10 @@
         <v>56</v>
       </c>
       <c r="G303">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H303">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I303" t="s">
         <v>45</v>
@@ -12995,10 +12995,10 @@
         <v>56</v>
       </c>
       <c r="G304">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H304">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I304" t="s">
         <v>45</v>
@@ -13036,10 +13036,10 @@
         <v>56</v>
       </c>
       <c r="G305">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H305">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I305" t="s">
         <v>45</v>
@@ -13077,10 +13077,10 @@
         <v>56</v>
       </c>
       <c r="G306">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H306">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I306" t="s">
         <v>45</v>
@@ -13118,10 +13118,10 @@
         <v>56</v>
       </c>
       <c r="G307">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H307">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I307" t="s">
         <v>45</v>
@@ -13159,10 +13159,10 @@
         <v>56</v>
       </c>
       <c r="G308">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H308">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I308" t="s">
         <v>45</v>
@@ -13200,10 +13200,10 @@
         <v>56</v>
       </c>
       <c r="G309">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H309">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I309" t="s">
         <v>45</v>
@@ -13241,10 +13241,10 @@
         <v>56</v>
       </c>
       <c r="G310">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H310">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I310" t="s">
         <v>45</v>
@@ -13282,10 +13282,10 @@
         <v>56</v>
       </c>
       <c r="G311">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H311">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I311" t="s">
         <v>45</v>
@@ -13323,10 +13323,10 @@
         <v>56</v>
       </c>
       <c r="G312">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H312">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I312" t="s">
         <v>45</v>
@@ -13364,10 +13364,10 @@
         <v>56</v>
       </c>
       <c r="G313">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H313">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I313" t="s">
         <v>45</v>
@@ -13405,10 +13405,10 @@
         <v>56</v>
       </c>
       <c r="G314">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H314">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I314" t="s">
         <v>45</v>
@@ -13446,10 +13446,10 @@
         <v>56</v>
       </c>
       <c r="G315">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H315">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I315" t="s">
         <v>45</v>
@@ -13487,10 +13487,10 @@
         <v>56</v>
       </c>
       <c r="G316">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H316">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I316" t="s">
         <v>45</v>
@@ -13528,10 +13528,10 @@
         <v>56</v>
       </c>
       <c r="G317">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H317">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I317" t="s">
         <v>45</v>
@@ -13569,10 +13569,10 @@
         <v>56</v>
       </c>
       <c r="G318">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H318">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I318" t="s">
         <v>45</v>
@@ -13610,10 +13610,10 @@
         <v>56</v>
       </c>
       <c r="G319">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H319">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I319" t="s">
         <v>45</v>
@@ -13651,10 +13651,10 @@
         <v>56</v>
       </c>
       <c r="G320">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H320">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I320" t="s">
         <v>45</v>
@@ -13692,10 +13692,10 @@
         <v>56</v>
       </c>
       <c r="G321">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H321">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I321" t="s">
         <v>45</v>
@@ -13733,10 +13733,10 @@
         <v>56</v>
       </c>
       <c r="G322">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H322">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I322" t="s">
         <v>45</v>
@@ -13774,10 +13774,10 @@
         <v>56</v>
       </c>
       <c r="G323">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H323">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I323" t="s">
         <v>45</v>
@@ -13815,10 +13815,10 @@
         <v>56</v>
       </c>
       <c r="G324">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H324">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I324" t="s">
         <v>45</v>
@@ -13856,10 +13856,10 @@
         <v>56</v>
       </c>
       <c r="G325">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H325">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I325" t="s">
         <v>45</v>
@@ -13897,10 +13897,10 @@
         <v>56</v>
       </c>
       <c r="G326">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H326">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I326" t="s">
         <v>45</v>
@@ -13938,10 +13938,10 @@
         <v>56</v>
       </c>
       <c r="G327">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H327">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I327" t="s">
         <v>45</v>
@@ -13979,10 +13979,10 @@
         <v>56</v>
       </c>
       <c r="G328">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H328">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I328" t="s">
         <v>45</v>
@@ -14020,10 +14020,10 @@
         <v>56</v>
       </c>
       <c r="G329">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H329">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I329" t="s">
         <v>45</v>
@@ -14061,10 +14061,10 @@
         <v>56</v>
       </c>
       <c r="G330">
-        <v>46.85230749999999</v>
+        <v>46.8799663</v>
       </c>
       <c r="H330">
-        <v>-121.7603229</v>
+        <v>-121.7269094</v>
       </c>
       <c r="I330" t="s">
         <v>45</v>

</xml_diff>